<commit_message>
feat: se termina seccion de impresion de etiquetas
Utilizando axios se envia un post para imprimir etiquetas
</commit_message>
<xml_diff>
--- a/Label/Programa_Produccion.xlsx
+++ b/Label/Programa_Produccion.xlsx
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="6" uniqueCount="6">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="40" uniqueCount="40">
   <si>
     <t>cantidad</t>
   </si>
@@ -42,6 +42,108 @@
   </si>
   <si>
     <t>Linea</t>
+  </si>
+  <si>
+    <t>5E0005207202</t>
+  </si>
+  <si>
+    <t>5000012188A0</t>
+  </si>
+  <si>
+    <t>5E0005304584</t>
+  </si>
+  <si>
+    <t>5E0005304395</t>
+  </si>
+  <si>
+    <t>5E0005304396</t>
+  </si>
+  <si>
+    <t>5000010462A0</t>
+  </si>
+  <si>
+    <t>5000010464A0</t>
+  </si>
+  <si>
+    <t>5000010466A0</t>
+  </si>
+  <si>
+    <t>5000010484A0</t>
+  </si>
+  <si>
+    <t>5000010482A0</t>
+  </si>
+  <si>
+    <t>5000010473A0</t>
+  </si>
+  <si>
+    <t>5000010479A0</t>
+  </si>
+  <si>
+    <t>5000010477A0</t>
+  </si>
+  <si>
+    <t>5E0005304293</t>
+  </si>
+  <si>
+    <t>5E0005304294</t>
+  </si>
+  <si>
+    <t>5E0005304285</t>
+  </si>
+  <si>
+    <t>5E0005304286</t>
+  </si>
+  <si>
+    <t>5E0005304295</t>
+  </si>
+  <si>
+    <t>5E0005304296</t>
+  </si>
+  <si>
+    <t>5E0005304287</t>
+  </si>
+  <si>
+    <t>5E0005304289</t>
+  </si>
+  <si>
+    <t>5E0005304290</t>
+  </si>
+  <si>
+    <t>5E0005304291</t>
+  </si>
+  <si>
+    <t>5E0005304297</t>
+  </si>
+  <si>
+    <t>5E0005304298</t>
+  </si>
+  <si>
+    <t>5E0005304299</t>
+  </si>
+  <si>
+    <t>5E0005304300</t>
+  </si>
+  <si>
+    <t>5E0005304301</t>
+  </si>
+  <si>
+    <t>5E0005304302</t>
+  </si>
+  <si>
+    <t>5E0005304359</t>
+  </si>
+  <si>
+    <t>5E0005304360</t>
+  </si>
+  <si>
+    <t>5E0005304361</t>
+  </si>
+  <si>
+    <t>5E0005304362</t>
+  </si>
+  <si>
+    <t>5E0005304340</t>
   </si>
 </sst>
 </file>
@@ -360,10 +462,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:C4"/>
+  <dimension ref="A1:C38"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C9" sqref="C9"/>
+      <selection activeCell="E29" sqref="E29"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -418,6 +520,380 @@
         <v>3</v>
       </c>
     </row>
+    <row r="5" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A5" t="s">
+        <v>6</v>
+      </c>
+      <c r="B5">
+        <v>1300</v>
+      </c>
+      <c r="C5">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="6" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A6" t="s">
+        <v>7</v>
+      </c>
+      <c r="B6">
+        <v>1600</v>
+      </c>
+      <c r="C6">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="7" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A7" t="s">
+        <v>8</v>
+      </c>
+      <c r="B7">
+        <v>1500</v>
+      </c>
+      <c r="C7">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="8" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A8" t="s">
+        <v>9</v>
+      </c>
+      <c r="B8">
+        <v>2000</v>
+      </c>
+      <c r="C8">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="9" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A9" t="s">
+        <v>10</v>
+      </c>
+      <c r="B9">
+        <v>1500</v>
+      </c>
+      <c r="C9">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="10" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A10" t="s">
+        <v>11</v>
+      </c>
+      <c r="B10">
+        <v>1300</v>
+      </c>
+      <c r="C10">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="11" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A11" t="s">
+        <v>12</v>
+      </c>
+      <c r="B11">
+        <v>1600</v>
+      </c>
+      <c r="C11">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="12" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A12" t="s">
+        <v>13</v>
+      </c>
+      <c r="B12">
+        <v>1500</v>
+      </c>
+      <c r="C12">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="13" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A13" t="s">
+        <v>14</v>
+      </c>
+      <c r="B13">
+        <v>2000</v>
+      </c>
+      <c r="C13">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="14" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A14" t="s">
+        <v>15</v>
+      </c>
+      <c r="B14">
+        <v>1500</v>
+      </c>
+      <c r="C14">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="15" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A15" t="s">
+        <v>16</v>
+      </c>
+      <c r="B15">
+        <v>1300</v>
+      </c>
+      <c r="C15">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="16" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A16" t="s">
+        <v>17</v>
+      </c>
+      <c r="B16">
+        <v>1600</v>
+      </c>
+      <c r="C16">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="17" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A17" t="s">
+        <v>18</v>
+      </c>
+      <c r="B17">
+        <v>1500</v>
+      </c>
+      <c r="C17">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="18" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A18" t="s">
+        <v>19</v>
+      </c>
+      <c r="B18">
+        <v>2000</v>
+      </c>
+      <c r="C18">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="19" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A19" t="s">
+        <v>20</v>
+      </c>
+      <c r="B19">
+        <v>1500</v>
+      </c>
+      <c r="C19">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="20" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A20" t="s">
+        <v>21</v>
+      </c>
+      <c r="B20">
+        <v>1300</v>
+      </c>
+      <c r="C20">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="21" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A21" t="s">
+        <v>22</v>
+      </c>
+      <c r="B21">
+        <v>1600</v>
+      </c>
+      <c r="C21">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="22" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A22" t="s">
+        <v>23</v>
+      </c>
+      <c r="B22">
+        <v>1500</v>
+      </c>
+      <c r="C22">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="23" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A23" t="s">
+        <v>24</v>
+      </c>
+      <c r="B23">
+        <v>2000</v>
+      </c>
+      <c r="C23">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="24" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A24" t="s">
+        <v>25</v>
+      </c>
+      <c r="B24">
+        <v>1500</v>
+      </c>
+      <c r="C24">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="25" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A25" t="s">
+        <v>26</v>
+      </c>
+      <c r="B25">
+        <v>1300</v>
+      </c>
+      <c r="C25">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="26" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A26" t="s">
+        <v>27</v>
+      </c>
+      <c r="B26">
+        <v>1600</v>
+      </c>
+      <c r="C26">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="27" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A27" t="s">
+        <v>28</v>
+      </c>
+      <c r="B27">
+        <v>1500</v>
+      </c>
+      <c r="C27">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="28" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A28" t="s">
+        <v>29</v>
+      </c>
+      <c r="B28">
+        <v>2000</v>
+      </c>
+      <c r="C28">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="29" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A29" t="s">
+        <v>30</v>
+      </c>
+      <c r="B29">
+        <v>1500</v>
+      </c>
+      <c r="C29">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="30" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A30" t="s">
+        <v>31</v>
+      </c>
+      <c r="B30">
+        <v>1300</v>
+      </c>
+      <c r="C30">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="31" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A31" t="s">
+        <v>32</v>
+      </c>
+      <c r="B31">
+        <v>1600</v>
+      </c>
+      <c r="C31">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="32" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A32" t="s">
+        <v>33</v>
+      </c>
+      <c r="B32">
+        <v>1500</v>
+      </c>
+      <c r="C32">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="33" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A33" t="s">
+        <v>34</v>
+      </c>
+      <c r="B33">
+        <v>2000</v>
+      </c>
+      <c r="C33">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="34" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A34" t="s">
+        <v>35</v>
+      </c>
+      <c r="B34">
+        <v>1500</v>
+      </c>
+      <c r="C34">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="35" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A35" t="s">
+        <v>36</v>
+      </c>
+      <c r="B35">
+        <v>1300</v>
+      </c>
+      <c r="C35">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="36" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A36" t="s">
+        <v>37</v>
+      </c>
+      <c r="B36">
+        <v>1600</v>
+      </c>
+      <c r="C36">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="37" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A37" t="s">
+        <v>38</v>
+      </c>
+      <c r="B37">
+        <v>1000</v>
+      </c>
+      <c r="C37">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="38" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A38" t="s">
+        <v>39</v>
+      </c>
+      <c r="B38">
+        <v>2000</v>
+      </c>
+      <c r="C38">
+        <v>2</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>

</xml_diff>

<commit_message>
Cambio de proceso de base de datos a SAP
</commit_message>
<xml_diff>
--- a/Label/Programa_Produccion.xlsx
+++ b/Label/Programa_Produccion.xlsx
@@ -5,11 +5,11 @@
   <workbookPr defaultThemeVersion="164011"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\aram.guillen\Documents\GitHub\extrusion\label\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\aram.guillen\Documents\GitHub\extrusion\Label\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="12450"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="18345" windowHeight="7665"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="7" uniqueCount="6">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="6" uniqueCount="6">
   <si>
     <t>5000010103A0</t>
   </si>
@@ -360,10 +360,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:C5"/>
+  <dimension ref="A1:C4"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C2" sqref="C2"/>
+      <selection activeCell="C6" sqref="C6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -390,7 +390,7 @@
         <v>0</v>
       </c>
       <c r="B2">
-        <v>100</v>
+        <v>4500</v>
       </c>
       <c r="C2">
         <v>1</v>
@@ -401,7 +401,7 @@
         <v>1</v>
       </c>
       <c r="B3">
-        <v>100</v>
+        <v>1000</v>
       </c>
       <c r="C3">
         <v>1</v>
@@ -412,20 +412,9 @@
         <v>3</v>
       </c>
       <c r="B4">
-        <v>100</v>
+        <v>1000</v>
       </c>
       <c r="C4">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="5" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A5" t="s">
-        <v>3</v>
-      </c>
-      <c r="B5">
-        <v>100</v>
-      </c>
-      <c r="C5">
         <v>2</v>
       </c>
     </row>

</xml_diff>